<commit_message>
indexing added to save
</commit_message>
<xml_diff>
--- a/persistance/data/New_ASINS.xlsx
+++ b/persistance/data/New_ASINS.xlsx
@@ -495,16 +495,16 @@
         </is>
       </c>
       <c r="F2" t="n">
-        <v>0.3285377975411981</v>
+        <v>0</v>
       </c>
       <c r="J2" t="n">
         <v>-100</v>
       </c>
       <c r="K2" t="n">
-        <v>12.56</v>
+        <v>0</v>
       </c>
       <c r="L2" t="n">
-        <v>38.23</v>
+        <v>137.82</v>
       </c>
       <c r="M2" t="n">
         <v>0</v>
@@ -518,6 +518,24 @@
         <is>
           <t>B01JLPJM7G</t>
         </is>
+      </c>
+      <c r="F3" t="n">
+        <v>0.3293130571578395</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-100</v>
+      </c>
+      <c r="K3" t="n">
+        <v>12.56</v>
+      </c>
+      <c r="L3" t="n">
+        <v>38.14</v>
+      </c>
+      <c r="M3" t="n">
+        <v>0</v>
+      </c>
+      <c r="N3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="4">

</xml_diff>